<commit_message>
added code to read excel files
</commit_message>
<xml_diff>
--- a/testData/users.xlsx
+++ b/testData/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/everst/Documents/w2a/playwright-session/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFDA3A99-E415-9F4D-A5C0-CD31D2764B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8CAF1D-D65F-744F-866C-9C663A44CD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15640" xr2:uid="{74D7F270-EEB5-494A-A56F-FA6E98CA8702}"/>
   </bookViews>
@@ -44,12 +44,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>password1</t>
-  </si>
-  <si>
     <t>user2</t>
   </si>
   <si>
@@ -72,13 +66,19 @@
   </si>
   <si>
     <t>password5</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>standard_user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,6 +91,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,8 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +439,13 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="23.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -445,44 +455,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>